<commit_message>
Correccion documento casos de prueba
</commit_message>
<xml_diff>
--- a/Documentos de prueba/Casos de prueba.xlsx
+++ b/Documentos de prueba/Casos de prueba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAURA MEJIA\Desktop\RetoChoucair\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAURA MEJIA\Desktop\RepoRetoChoucair\Documentos de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>ID_CASO</t>
   </si>
@@ -82,26 +82,12 @@
 ºIngresar al apartado de publicaciones y crear una </t>
   </si>
   <si>
-    <t xml:space="preserve">ºURL:https://s1.demo.opensourcecms.com/wordpress/wp-login.php
-ºUser:opensourcecms
-ºPassword:opensourcecms
-ºTitulo de la publicación: Prueba choucair
-ºTexto: Se realiza una publicación desde cero </t>
-  </si>
-  <si>
     <t>Certificar que la página permita editar una publicación ya creada</t>
   </si>
   <si>
     <t>ºIngresar a la URL
 ºIngresar las credenciales 
 º Ingresar al apartado de publicaciónes y editar una ya existente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ºURL:https://s1.demo.opensourcecms.com/wordpress/wp-login.php
-ºUser:opensourcecms
-ºPassword:opensourcecms
-ºTitulo:Prueba choucair 2
-ºTexto: Modificación del texto </t>
   </si>
   <si>
     <t>Validar que la plataforma permita realizar edición rapida en una publicación</t>
@@ -111,6 +97,69 @@
 ºUser:opensourcecms
 ºPassword:opensourcecms
 ºTitulo:Prueba choucair 3
+</t>
+  </si>
+  <si>
+    <t>Verificar que el post haya sido publicado correctamente</t>
+  </si>
+  <si>
+    <t>Verificar la actualización del post</t>
+  </si>
+  <si>
+    <t>CP005</t>
+  </si>
+  <si>
+    <t>CP006</t>
+  </si>
+  <si>
+    <t>Validar que la plataforma permita la creación de páginas</t>
+  </si>
+  <si>
+    <t>Certificar que la plataforma permite editar una página ya creada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ºURL:https://s1.demo.opensourcecms.com/wordpress/wp-login.php
+ºUser:opensourcecms
+ºPassword:opensourcecms
+ºTitulo de la publicación: Prueba choucair2
+ºTexto: Se realiza una publicación desde cero </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ºURL:https://s1.demo.opensourcecms.com/wordpress/wp-login.php
+ºUser:opensourcecms
+ºPassword:opensourcecms
+ºTitulo:Prueba choucair 25
+ºTexto: Modificación del texto </t>
+  </si>
+  <si>
+    <t>Verificar que la página fue publicada correctamente</t>
+  </si>
+  <si>
+    <t>Verificar la actualización de la página</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ºURL:https://s1.demo.opensourcecms.com/wordpress/wp-login.php
+ºUser:opensourcecms
+ºPassword:opensourcecms
+ºTitulo:Prueba choucair2
+ºUrl imagen:https://computacioninteractiva.com/wp-content/uploads/2019/07/INVERTIR-EN-TECNOLOGIA.png
+</t>
+  </si>
+  <si>
+    <t>ºIngresar a la URL
+ºIngresar las credenciales 
+º Ingresar al apartado de páginas y crear una</t>
+  </si>
+  <si>
+    <t>ºIngresar a la URL
+ºIngresar las credenciales 
+º Ingresar al apartado de páginas y editar una ya existente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ºURL:https://s1.demo.opensourcecms.com/wordpress/wp-login.php
+ºUser:opensourcecms
+ºPassword:opensourcecms
+ºTitulo:Prueba choucair25
 </t>
   </si>
 </sst>
@@ -192,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,6 +261,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -263,6 +318,158 @@
         <a:xfrm>
           <a:off x="6477000" y="942975"/>
           <a:ext cx="1580952" cy="380952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>300437</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2218773</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1333188</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6291662" y="2019300"/>
+          <a:ext cx="1918336" cy="1085538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>269921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2037855</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1342704</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6372226" y="3432221"/>
+          <a:ext cx="1656854" cy="1072783"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>97649</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3105151</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1523173</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6088874" y="5962650"/>
+          <a:ext cx="3007502" cy="1313623"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>93317</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3028950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1391513</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6084542" y="7534275"/>
+          <a:ext cx="2935633" cy="1162913"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -537,18 +744,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H7"/>
+  <dimension ref="A3:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="A10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
-    <col min="5" max="5" width="38" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -591,7 +798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -602,27 +809,31 @@
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
@@ -632,19 +843,59 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>